<commit_message>
Weapons continued + cherubim added
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Disciplines/Weapons.xlsx
+++ b/CoreRulebook/Data/Disciplines/Weapons.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$27</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$I$26</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="65">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -85,7 +85,7 @@
     <t xml:space="preserve">Stabbing</t>
   </si>
   <si>
-    <t xml:space="preserve">\imp{Concealed}, \imp{Poisoned}</t>
+    <t xml:space="preserve">Concealed, Poisoned, Thrown</t>
   </si>
   <si>
     <t xml:space="preserve">Club</t>
@@ -94,13 +94,13 @@
     <t xml:space="preserve">Spear</t>
   </si>
   <si>
-    <t xml:space="preserve">Can be thrown (see \imp{Javelin})</t>
+    <t xml:space="preserve">Thrown</t>
   </si>
   <si>
     <t xml:space="preserve">Knuckleduster</t>
   </si>
   <si>
-    <t xml:space="preserve">\imp{Concealed}</t>
+    <t xml:space="preserve">Concealed, Poisoned</t>
   </si>
   <si>
     <t xml:space="preserve">Whip</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">Cutting</t>
   </si>
   <si>
-    <t xml:space="preserve">Can initiate \imp{Grapple}</t>
+    <t xml:space="preserve">Grapple</t>
   </si>
   <si>
     <t xml:space="preserve">Axe</t>
@@ -130,13 +130,13 @@
     <t xml:space="preserve">Any Physical</t>
   </si>
   <si>
-    <t xml:space="preserve">Two-handed, \imp{Cumbersome}</t>
+    <t xml:space="preserve">Two-handed, cumbersome</t>
   </si>
   <si>
     <t xml:space="preserve">Kama</t>
   </si>
   <si>
-    <t xml:space="preserve">In pair, +1 DV, +1 damage</t>
+    <t xml:space="preserve">Paired</t>
   </si>
   <si>
     <t xml:space="preserve">Greataxe</t>
@@ -166,9 +166,6 @@
     <t xml:space="preserve">Shortbow</t>
   </si>
   <si>
-    <t xml:space="preserve">Javelin</t>
-  </si>
-  <si>
     <t xml:space="preserve">Longbow</t>
   </si>
   <si>
@@ -178,40 +175,40 @@
     <t xml:space="preserve">Reload (1)</t>
   </si>
   <si>
-    <t xml:space="preserve">Revolver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reload (6), \imp{Concealed}</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pistol</t>
   </si>
   <si>
-    <t xml:space="preserve">Reload (8),  \imp{Concealed}</t>
+    <t xml:space="preserve">Reload (8), Concealed</t>
   </si>
   <si>
     <t xml:space="preserve">Rifle</t>
   </si>
   <si>
+    <t xml:space="preserve">Reload (1), Two-handed</t>
+  </si>
+  <si>
     <t xml:space="preserve">Semi-Auto Rifle</t>
   </si>
   <si>
-    <t xml:space="preserve">Reload (10)</t>
+    <t xml:space="preserve">Reload (10), Two-handed</t>
   </si>
   <si>
     <t xml:space="preserve">Shotgun</t>
   </si>
   <si>
+    <t xml:space="preserve">Reload (2), Two-handed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shotgun (Sawn-off)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reload (2)</t>
   </si>
   <si>
     <t xml:space="preserve">Machine Gun</t>
   </si>
   <si>
-    <t xml:space="preserve">1–4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reload (25), Variable Fire (+1 damage per 5 bullets, min 5)</t>
+    <t xml:space="preserve">Reload (5), Burst Fire, Two-handed</t>
   </si>
   <si>
     <t xml:space="preserve">Sniper Rifle</t>
@@ -220,23 +217,7 @@
     <t xml:space="preserve">Extreme</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Reload (1), </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">\imp{Cumbersome}</t>
-    </r>
+    <t xml:space="preserve">Reload (1), Cumbersome, Two-handed</t>
   </si>
 </sst>
 </file>
@@ -246,7 +227,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -267,11 +248,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -346,10 +322,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -615,6 +591,9 @@
       <c r="H9" s="0" t="s">
         <v>27</v>
       </c>
+      <c r="I9" s="0" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
@@ -839,7 +818,7 @@
         <v>19</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -850,7 +829,7 @@
         <v>42</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>44</v>
@@ -876,19 +855,19 @@
         <v>42</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>44</v>
       </c>
       <c r="E19" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F19" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H19" s="0" t="s">
         <v>19</v>
@@ -902,27 +881,30 @@
         <v>42</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>44</v>
       </c>
       <c r="E20" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F20" s="0" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G20" s="0" t="n">
         <v>2</v>
       </c>
       <c r="H20" s="0" t="s">
         <v>19</v>
+      </c>
+      <c r="I20" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>42</v>
@@ -934,10 +916,10 @@
         <v>44</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F21" s="0" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G21" s="0" t="n">
         <v>2</v>
@@ -946,47 +928,47 @@
         <v>19</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>44</v>
       </c>
       <c r="E22" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F22" s="0" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H22" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>44</v>
@@ -998,24 +980,24 @@
         <v>7</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H23" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D24" s="0" t="s">
         <v>44</v>
@@ -1024,27 +1006,27 @@
         <v>3</v>
       </c>
       <c r="F24" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H24" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="D25" s="0" t="s">
         <v>44</v>
@@ -1053,107 +1035,78 @@
         <v>3</v>
       </c>
       <c r="F25" s="0" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H25" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="D26" s="0" t="s">
         <v>44</v>
       </c>
       <c r="E26" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F26" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G26" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="G26" s="1" t="n">
         <v>4</v>
       </c>
       <c r="H26" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>42</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="D27" s="0" t="s">
         <v>44</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F27" s="0" t="n">
-        <v>6</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>61</v>
+        <v>10</v>
+      </c>
+      <c r="G27" s="0" t="n">
+        <v>8</v>
       </c>
       <c r="H27" s="0" t="s">
         <v>19</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="C28" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" s="0" t="n">
-        <v>5</v>
-      </c>
-      <c r="F28" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="G28" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>65</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I27"/>
+  <autoFilter ref="A1:I26"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>